<commit_message>
delete blank cells (error) from excel file
blank cells (but included in the csv file) caused import error into phpMyAdmin database tool.

* delete 4 blank columns after the last data column in the table
</commit_message>
<xml_diff>
--- a/support files/raw excel files/food_data.xlsx
+++ b/support files/raw excel files/food_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroof\OneDrive - Massey High School\Documents\Databases\L2\L2_DB_Assessment\support files\raw excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B548FE4-F4A5-4D16-872B-88F31481D78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D805608-4D64-4D8E-BD10-FBE8950D0923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{DA8D756B-AB59-47C8-AA2D-A3C8E430418F}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{DA8D756B-AB59-47C8-AA2D-A3C8E430418F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="calorie chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="167">
   <si>
     <t>ID</t>
   </si>
@@ -523,13 +524,28 @@
   </si>
   <si>
     <t>Vanilla Shake</t>
+  </si>
+  <si>
+    <t>Lower Quartile</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Upper Quartile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,16 +561,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -562,16 +611,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,6 +711,1601 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Calories content</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(all meals sorted from most to least calories)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'calorie chart'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calories</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'calorie chart'!$A$2:$A$243</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="242"/>
+                <c:pt idx="0">
+                  <c:v>1880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB0B-4F57-B3D5-A4718DD29A84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="604527152"/>
+        <c:axId val="604527568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="604527152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="604527568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="604527568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="604527152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>493778</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>236322</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>75067</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38432D67-7D24-46A7-8A21-0E593F852697}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -886,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0781B625-6820-4221-8B9A-BD1F911DB4A8}">
   <dimension ref="A1:R241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:R241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11522,4 +13243,1260 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4673697-55AF-4125-AD95-DFC66AF0DDAF}">
+  <dimension ref="A1:D241"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1090</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1050</v>
+      </c>
+      <c r="D5" s="4">
+        <f>QUARTILE(A2:A250,1)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>990</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>940</v>
+      </c>
+      <c r="D7" s="4">
+        <f>MEDIAN(A:A)</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>930</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>850</v>
+      </c>
+      <c r="D9" s="4">
+        <f>QUARTILE(A:A,3)</f>
+        <v>502.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>820</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>820</v>
+      </c>
+      <c r="D11" s="6">
+        <f>AVERAGE(A:A)</f>
+        <v>370.1875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A242">
+    <sortCondition descending="1" ref="A2:A242"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>